<commit_message>
Adding iterative improvement Heuristics
</commit_message>
<xml_diff>
--- a/bee_simulation_results.xlsx
+++ b/bee_simulation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Path</t>
+          <t>Path Indices</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total Distance</t>
+          <t>Distance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Path Coordinates</t>
         </is>
       </c>
     </row>
@@ -456,11 +461,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (4, -4) -&gt; (0, -12)</t>
+          <t>0 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>77.05240967118867</v>
+        <v>271.1083505599865</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[(0, -12), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, 12), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -469,11 +479,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 0</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>81.88854381999832</v>
+        <v>67.77708763999664</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -482,11 +497,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>81.88854381999832</v>
+        <v>107.7770876399966</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (4, -4), (4, 12), (4, -4), (-4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -495,11 +515,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (0, 20) -&gt; (-4, 12) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>75.16386585119035</v>
+        <v>101.665631459995</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (4, 12), (4, -4), (-4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -508,11 +533,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>81.88854381999832</v>
+        <v>105.8885438199983</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (4, 12), (4, -4), (4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -521,11 +551,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 0</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>81.88854381999832</v>
+        <v>100.4391878823824</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (0, 20), (4, 12), (4, -4), (-4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -534,11 +569,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (0, 20) -&gt; (-4, 12) -&gt; (4, 12) -&gt; (4, -4) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 0</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>75.16386585119035</v>
+        <v>77.05240967118867</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (4, -4), (-4, 12), (0, 20), (4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -547,11 +587,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 0</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>81.88854381999832</v>
+        <v>67.77708763999664</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -560,11 +605,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 3 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 3 -&gt; 4 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>81.88854381999832</v>
+        <v>168.216275522379</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>[(0, -12), (0, 20), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, 20), (4, 12), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -573,11 +623,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>81.88854381999832</v>
+        <v>101.665631459995</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (4, 12), (4, -4), (-4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -586,11 +641,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 0</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>81.88854381999832</v>
+        <v>67.77708763999664</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -599,11 +659,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>81.88854381999832</v>
+        <v>193.4427190999916</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>[(0, -12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (4, 12), (4, -4), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -612,11 +677,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>81.88854381999832</v>
+        <v>71.55417527999327</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[(0, -12), (4, -4), (-4, 12), (0, 20), (4, 12), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -625,11 +695,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 0</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>81.88854381999832</v>
+        <v>132.4391878823824</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (0, 20), (4, 12), (4, -4), (4, 12), (4, -4), (-4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -638,11 +713,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 0</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>81.88854381999832</v>
+        <v>77.05240967118867</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (4, -4), (-4, 12), (0, 20), (4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -651,11 +731,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 0</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>81.88854381999832</v>
+        <v>67.77708763999664</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -664,11 +749,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>81.88854381999832</v>
+        <v>126.940953491187</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -677,11 +767,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (4, -4) -&gt; (-4, -4) -&gt; (-4, 12) -&gt; (4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>81.88854381999832</v>
+        <v>233.4915975535711</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>[(0, -12), (4, 12), (4, -4), (4, 12), (4, -4), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -690,11 +785,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 0</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>81.88854381999832</v>
+        <v>118.3277317023807</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, -4), (-4, 12), (0, 20), (4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -703,11 +803,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>81.88854381999832</v>
+        <v>171.7770876399966</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (4, -4), (4, 12), (4, -4), (4, 12), (4, -4), (-4, -4), (-4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -716,11 +821,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (-4, 12) -&gt; (4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 5 -&gt; 3 -&gt; 4 -&gt; 0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>83.77708763999664</v>
+        <v>100.4391878823824</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (4, -4), (0, 20), (4, 12), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -729,11 +839,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 5 -&gt; 2 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>81.88854381999832</v>
+        <v>113.4427190999916</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>[(0, -12), (4, -4), (-4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -742,11 +857,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 1 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 0</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>81.88854381999832</v>
+        <v>139.7770876399966</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (-4, -4), (4, 12), (4, -4), (-4, -4), (-4, 12), (0, 20), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -755,11 +875,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
+          <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 0</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>81.88854381999832</v>
+        <v>119.5541752799933</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, -4), (-4, 12), (0, 20), (4, 12), (-4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -768,76 +893,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (4, -4) -&gt; (0, -12)</t>
+          <t>0 -&gt; 2 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 1 -&gt; 0</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>77.05240967118867</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>81.88854381999832</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>81.88854381999832</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>81.88854381999832</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>81.88854381999832</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>(0, -12) -&gt; (-4, -4) -&gt; (4, -4) -&gt; (4, 12) -&gt; (-4, 12) -&gt; (0, 20) -&gt; (0, -12)</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>81.88854381999832</v>
+        <v>162.7180411311836</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>[(0, -12), (-4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, 12), (0, 20), (4, 12), (4, -4), (-4, -4), (0, -12)]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>